<commit_message>
continue write testcase for genisoimage and test root 34
</commit_message>
<xml_diff>
--- a/packages_testcase.xlsx
+++ b/packages_testcase.xlsx
@@ -146,61 +146,6 @@
         <rFont val="Verdana"/>
         <family val="2"/>
       </rPr>
-      <t>1, 2, 4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. Create directory "cd_dir" for testing.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">3. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Create files "file1, file2, file3" for testing.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t>4.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Install wodim package.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
       <t>1.</t>
     </r>
     <r>
@@ -305,7 +250,142 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Create a HFS hybrid CD with the Joliet and Rock Ridge extensions of the source directory cd_dir:
-# genisoimage -o cd.iso -R -J -hfs cd_dir</t>
+# genisoimage -o cd.iso -R -J -hfs cd_dir
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>7.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Read ISO-9660 image from SCSI target to use as CD/DVD-Recorder:
+# devdump -i cd.iso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>8.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Split a folder containing thousands of files totaling up to more than 700MB into individual directories of 700 MB each - ready for burning onto multiple CDs:
+# dirsplit --size 700M --expmode 1 allimages/
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>9.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Extract an El Torito image from a 
+bootable CD (or cd-image) and write the data extracted to a file:
+# geteltorito -o eltorito debian-9.3.0-amd64-netinst.iso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Read ISO-9660 image from SCSI target to use as CD/DVD-Recorder:
+# isodump -i cd.iso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>11.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Read ISO-9660 image from SCSI target and print information from the primary volume descriptor:
+# isoinfo -d -i debian-9.3.0-amd64-netinst.iso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>12.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Verify the integrity of the specified ISO9660 image and write the results to standard output:
+# isovfy -i cd.iso 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>13.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Create a zisofs/RockRidge compressed file tree:
+# mkzftree -p 9 --one-filesystem allimages/ img_compressed
+</t>
     </r>
   </si>
   <si>
@@ -533,6 +613,358 @@
 Max brk space used 0
 591 extents written (1 MB)
 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>7.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Get output like:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">00000000 00000000 00000000 00000000 00000000 ................
+00000010 00000000 00000000 00000000 00000000 ................
+00000020 00000000 00000000 00000000 00000000 ................
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>8.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Get output like:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Building file list, please wait...
+Calculating, please wait...
+....................
+Calculated, using 2 volumes.
+Wasted: 13 Byte (estimated, check mkisofs -print-size ...)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>9.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Get output like:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Booting catalog starts at sector: 939 
+Manufacturer of CD: 
+Image architecture: x86
+Boot media type is: no emulation
+El Torito image starts at sector 1148 and has 4 sector(s) of 512 Bytes
+Image has been written to file "eltorito".</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Get output like:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 34 [ 1]    17     2048 02/*.             
+ 34 [ 1]    17     2048 02/*..            
+ Zone, zone offset:     17 0000  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>11.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Get output like:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CD-ROM is in ISO 9660 format
+System id: 
+Volume id: Debian 9.3.0 amd64 n
+Volume set id: 
+Publisher id: 
+Data preparer id: XORRISO-1.4.6 2016.09.16.133001, LIBISOBURN-1.4.6, LIBISOFS-1.4.6, LIBBURN-1.4.6
+Application id: 
+Copyright File id: 
+Abstract File id: 
+Bibliographic File id: 
+Volume set size is: 1
+Volume set sequence number is: 1
+Logical block size is: 2048
+Volume size is: 148480
+El Torito VD version 1 found, boot catalog is in sector 939
+Joliet with UCS level 3 found
+Rock Ridge signatures version 1 found
+Eltorito validation header:
+    Hid 1
+    Arch 0 (x86)
+    ID ''
+    Key 55 AA
+    Eltorito defaultboot header:
+        Bootid 88 (bootable)
+        Boot media 0 (No Emulation Boot)
+        Load segment 0
+        Sys type 0
+        Nsect 4
+        Bootoff 47C 1148
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>12.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Get output like:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Root at extent 1c, 2048 bytes
+[0 0]
+No errors found</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>13.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> No output. A compressed file tree was created.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>1, 2, 3, 4, 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Create a directory "cd_dir" for testing.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Create files "file1, file2, file3" for testing.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>7, 10, 12.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Create "cd.iso" for testing.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>8, 13.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Create a directory "allimages" with more than 700MB data.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>9, 11.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Prepare a bootable CD (or cd-image).</t>
     </r>
   </si>
 </sst>
@@ -891,7 +1323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -933,13 +1365,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>

</xml_diff>